<commit_message>
party vessels catch script and minor changes to some xlsx
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb129/raw/Table23.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb129/raw/Table23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb129/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BF486E-9740-2F4F-B214-24A666ACC237}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B050F1-DA1D-8845-90BA-29071B30E67D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,35 +30,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Species</t>
   </si>
   <si>
-    <t>Total number of fish____________________________</t>
-  </si>
-  <si>
-    <t>Tuna albacore__________________________________</t>
-  </si>
-  <si>
     <t>Barracuda Gdfotua</t>
   </si>
   <si>
     <t>Bass kelp and sand</t>
   </si>
   <si>
-    <t>Bonito Pacific_____________</t>
-  </si>
-  <si>
-    <t>Halibut California______</t>
-  </si>
-  <si>
     <t>Lingcod</t>
   </si>
   <si>
-    <t>Mackerel jack______________________</t>
-  </si>
-  <si>
     <t>Mackerel Pacific</t>
   </si>
   <si>
@@ -68,37 +53,55 @@
     <t>Salmon</t>
   </si>
   <si>
-    <t>Scul pin</t>
-  </si>
-  <si>
     <t>Seabasa white</t>
   </si>
   <si>
-    <t>Sheepbead California______________'</t>
-  </si>
-  <si>
     <t>Tuna bluefin</t>
   </si>
   <si>
     <t>Whitefish ocean</t>
   </si>
   <si>
-    <t>Yellow-tail California____</t>
-  </si>
-  <si>
     <t>All others</t>
   </si>
   <si>
     <t>Total check</t>
   </si>
   <si>
-    <t>Number of angler days__________________________</t>
-  </si>
-  <si>
     <t>Number of anglers</t>
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Bonito Pacific</t>
+  </si>
+  <si>
+    <t>Halibut California</t>
+  </si>
+  <si>
+    <t>Mackerel jack</t>
+  </si>
+  <si>
+    <t>Sheepbead California</t>
+  </si>
+  <si>
+    <t>Cabezon</t>
+  </si>
+  <si>
+    <t>Total number of fish</t>
+  </si>
+  <si>
+    <t>Number of angler days</t>
+  </si>
+  <si>
+    <t>Sculpin</t>
+  </si>
+  <si>
+    <t>Tuna albacore</t>
+  </si>
+  <si>
+    <t>Yellowtail California</t>
   </si>
 </sst>
 </file>
@@ -532,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -584,7 +587,7 @@
     </row>
     <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="7">
         <v>282552</v>
@@ -619,7 +622,7 @@
     </row>
     <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7">
         <v>876667</v>
@@ -652,9 +655,9 @@
         <v>1219344</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B4" s="10">
         <v>70078</v>
@@ -688,7 +691,9 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
+      <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="B5" s="10">
         <v>13132</v>
       </c>
@@ -720,9 +725,9 @@
         <v>9726</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B6" s="10">
         <v>59674</v>
@@ -757,7 +762,7 @@
     </row>
     <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B7" s="7">
         <v>22940</v>
@@ -790,9 +795,9 @@
         <v>27513</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B8" s="10">
         <v>19407</v>
@@ -827,7 +832,7 @@
     </row>
     <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B9" s="10">
         <v>315037</v>
@@ -862,7 +867,7 @@
     </row>
     <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10" s="10">
         <v>1149367</v>
@@ -897,7 +902,7 @@
     </row>
     <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B11" s="10">
         <v>119911</v>
@@ -932,7 +937,7 @@
     </row>
     <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B12" s="7">
         <v>33462</v>
@@ -967,7 +972,7 @@
     </row>
     <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B13" s="7">
         <v>41588</v>
@@ -1000,9 +1005,9 @@
         <v>19800</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B14" s="10">
         <v>21499</v>
@@ -1035,9 +1040,9 @@
         <v>18443</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B15" s="10">
         <v>20098</v>
@@ -1072,7 +1077,7 @@
     </row>
     <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B16" s="10">
         <v>966</v>
@@ -1107,7 +1112,7 @@
     </row>
     <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B17" s="7">
         <v>9952</v>
@@ -1140,9 +1145,9 @@
         <v>6231</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B18" s="10">
         <v>40872</v>
@@ -1177,7 +1182,7 @@
     </row>
     <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B19" s="10">
         <v>177335</v>
@@ -1210,9 +1215,9 @@
         <v>142630</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B20" s="10">
         <v>3274537</v>
@@ -1247,7 +1252,7 @@
     </row>
     <row r="21" spans="1:11" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A21" s="14" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B21" s="15">
         <f>SUM(B2:B19)-B20</f>
@@ -1290,7 +1295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1319,33 +1324,33 @@
         <v>495805</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H23" s="10">
         <v>637498</v>

</xml_diff>